<commit_message>
feat: Add web scraping, data cleaning, and WordPress data insertion with new API routes and authentication middleware.
</commit_message>
<xml_diff>
--- a/jobs.xlsx
+++ b/jobs.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -439,28 +439,28 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Trainee Conversion - Machine Learning Engineer</v>
+        <v>KAM - D2C Freight Operations</v>
       </c>
       <c r="B2" t="str">
-        <v>Bangalore, Karnataka, India</v>
+        <v>Chandigarh, Chandigarh, India</v>
       </c>
       <c r="C2" t="str">
-        <v>Mercedes Benz</v>
+        <v>Weekday</v>
       </c>
       <c r="D2" t="str">
-        <v>Global automotive research and development organization focusing on advanced engineering and innovative technologies.</v>
+        <v>A providing logistics and D2C freight management services.</v>
       </c>
       <c r="E2" t="str">
-        <v>https://kg.diffbot.com/image/api/get?fetch=yes&amp;urls=g%3Cj7P0SttAc%3ANu.d9U%7CB%5DpM08.%7DZnIa6%40_%3Bv2FpDLhawxEr-%5BuTpJZ%40-r%3Ec2Jh9e%3EN7%5Bt%3Be%3BNhDgx%7C%5BsC%5DBhn0d6PvRhxDp%5Bh.Pw4</v>
+        <v>https://kg.diffbot.com/image/api/get?fetch=yes&amp;urls=g%3Cj7P0Stn8p.%5DjEp9G.Bd%7Bk%3ESQLnc%7E%5B-AYYy-Z%3C%5BL-D%3A%7Bj-a%5CErs%3AwPm7S%5CzN_%3Cb4E.A%5Dm,g%3Cj7P0Stn8p.OgAu%3CRsCX3_1BY%2F%5Dt.%5B8LwifzFeCd.Nr0QoN%5CtW4BmCRh7%5E%7CZ-Oh1Cy6t%3Dm5Og.Z%5Et%60,g%3Cj7P0SttAc%3ANu.d9U%7CB%5DpM08.%7DZnIa6%40_%3Bv2FpDLhawxEr-%5BuTpJZ%40-r%3Ec2Jh9e%3ERjWglef5jxk%5DBa4MY%2Ftg</v>
       </c>
       <c r="F2" t="str">
-        <v>? YOEMaster in Computer/Electronics Engineering with focus on machine learning, computer vision, image processing or neural networks; strong C++, MATLAB, Lua skills; experience in computer vision and gesture recognition.</v>
+        <v>5+ YOE2+ MgmtEscalation management, client liaison, dashboards, NDR, COD remittance; 5+ years in D2C freight ops; leadership/account management experience; strong logistics knowledge.</v>
       </c>
       <c r="G2" t="str">
-        <v>C++, MATLAB, Lua, TensorFlow, Torch, Theano, Caffe, CUDA</v>
+        <v>Microsoft Excel</v>
       </c>
       <c r="H2" t="str">
-        <v>? YOE</v>
+        <v>5+ YOE</v>
       </c>
       <c r="I2" t="str">
         <v>Full Time</v>
@@ -469,152 +469,12 @@
         <v>Onsite</v>
       </c>
       <c r="K2" t="str">
-        <v>https://stgdaimler.taleo.net/careersection/ex/jobdetail.ftl?job=MER0001O8C&amp;lang=en</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>Associate Machine Learning Engineer</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Pakistan or India or United Arab Emirates or Australia or Canada or United States</v>
-      </c>
-      <c r="C3" t="str">
-        <v>VIDIZMO</v>
-      </c>
-      <c r="D3" t="str">
-        <v>A provider of video management and analytics software for enterprise customers.</v>
-      </c>
-      <c r="E3" t="str">
-        <v>https://kg.diffbot.com/image/api/get?fetch=yes&amp;urls=g%3Cj7P0Stn8p.OgAu%3CRsCX3_1BY%2F%5Dt.%5B8LwifzFeCd.Nr0QoN%5CtW4BmBVg5t8PYY%7DCa%3AZLqkX77Jf.9UsG,g%3Cj7P0Stn8p.%5DjEp9G.Bd%7Bk%3EZuOm9%7C%7D-fy%3B0-Z%3B%5CQ-D7%7CH-F%5DqSH%3Ar1ueN_zN_%3Cb4E.A%5Dm,g%3Cj7P0SttAc%3ANu.d9U%7CB%5DpM08.%7DZnIa6%40_%3Bv2FpDLhawxEr-%5BuTpJZ%40-r%3Ec2Jh9e%3E%5El9R6J%3C%2Flwl%7BFVGXx0S%3EW%7E%2FF0%3E4F%5CkYq</v>
-      </c>
-      <c r="F3" t="str">
-        <v>0+ YOEEntry-level to mid-level ML role; strong Python/C++/C#; experience with PyTorch/TensorFlow; CS degree; able to work independently; large data handling experience.</v>
-      </c>
-      <c r="G3" t="str">
-        <v>Python, C++, C#, OpenCV, PyTorch, TensorFlow</v>
-      </c>
-      <c r="H3" t="str">
-        <v>0+ YOE</v>
-      </c>
-      <c r="I3" t="str">
-        <v>Full Time</v>
-      </c>
-      <c r="J3" t="str">
-        <v>Hybrid</v>
-      </c>
-      <c r="K3" t="str">
-        <v>https://vidizmo.bamboohr.com/careers/341</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Machine Learning Intern</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Bangalore, Karnataka, India</v>
-      </c>
-      <c r="C4" t="str">
-        <v>Airbus</v>
-      </c>
-      <c r="D4" t="str">
-        <v>Global aerospace leader focused on innovation and cutting-edge technology.</v>
-      </c>
-      <c r="E4" t="str">
-        <v>https://kg.diffbot.com/image/api/get?fetch=yes&amp;urls=g%3Cj7P0SttAc%3ANu.d9U%7CB%5DpM08.%7DZnIa6%40_%3Bv2FpDLhawxEr-%5BuTpJZ%40-r%3Ec2Jh9e%3EN7%5Bu7k9NeIdx%7DT%7BZh%2F_l1m%3FG1Sm%3BAvDw.Vu4,g%3Cj7guSXzAoBWu.x0KwLZrUn.%5B%3CR0Aa4Hwygr9m6W%3Exl5G%60BkxmP%3E%60%7Ebv%7BF%3AHi7%7B%3FY%3D.%60%7CK,g%3Cj7P0St0DnBJf.x0KwLZrUn.%5B%3CR0Aa4Hh%3B%5Bv738ZqOr7U%3FgvFn%3EfW%3EOx%3FYdO%5EMl3Jo%3CLGg7LRwRXV-R%7DH_N%28P5Qe4%5D%7DJ%5B%3A%5B%29.Pw4</v>
-      </c>
-      <c r="F4" t="str">
-        <v>0+ YOEPursuing degree in CS/DS/Math/Engineering; strong Python; ML knowledge; ML frameworks; CV concepts; basic cloud and devops understanding.</v>
-      </c>
-      <c r="G4" t="str">
-        <v>TensorFlow, Keras, PyTorch, scikit-learn, Miniforge, VSCode, Git, AWS, Azure, Google Cloud, Docker, Kubernetes, SQL</v>
-      </c>
-      <c r="H4" t="str">
-        <v>0+ YOE</v>
-      </c>
-      <c r="I4" t="str">
-        <v/>
-      </c>
-      <c r="J4" t="str">
-        <v>Onsite</v>
-      </c>
-      <c r="K4" t="str">
-        <v>https://ag.wd3.myworkdayjobs.com/airbus/job/Bangalore-Area/Machine-Learning-Intern_JR10367255</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>AI Data Engineer (Bangalore, KA, IN)</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Bangalore, Karnataka, India</v>
-      </c>
-      <c r="C5" t="str">
-        <v>NTT Data</v>
-      </c>
-      <c r="D5" t="str">
-        <v>Global technology services provider</v>
-      </c>
-      <c r="E5" t="str">
-        <v>https://nttdata.com/global/en/-/media/assets/images/android-chrome-256256.png?rev=b1d7877f056340d181794ead6f1b3c16</v>
-      </c>
-      <c r="F5" t="str">
-        <v>? YOEAI Data Engineer with experience in machine learning, deep learning and GenAI.</v>
-      </c>
-      <c r="G5" t="str">
-        <v>Python, Machine Learning, Deep Learning, GenAI, LLM, Langchain</v>
-      </c>
-      <c r="H5" t="str">
-        <v>? YOE</v>
-      </c>
-      <c r="I5" t="str">
-        <v>Full Time</v>
-      </c>
-      <c r="J5" t="str">
-        <v>Onsite</v>
-      </c>
-      <c r="K5" t="str">
-        <v>https://careers-inc.nttdata.com/job/Bangalore-AI-Data-Engineer-KA/1233448100/</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>Technology and Transformation - EAD-AI/ML-Generative AI-Analyst (Bengaluru, IN)</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Bengaluru, Karnataka, India</v>
-      </c>
-      <c r="C6" t="str">
-        <v>Deloitte</v>
-      </c>
-      <c r="D6" t="str">
-        <v>Global professional services network delivering audit, tax, and consulting services that drive impact.</v>
-      </c>
-      <c r="E6" t="str">
-        <v>https://deloitte.com/content/dam/assets-shared/icons/us/favicon.ico</v>
-      </c>
-      <c r="F6" t="str">
-        <v>? YOEEntry-level data scientist or AI engineer focusing on building and deploying AI models; experience in data analysis, machine learning, or generative AI techniques.</v>
-      </c>
-      <c r="G6" t="str">
-        <v/>
-      </c>
-      <c r="H6" t="str">
-        <v>? YOE</v>
-      </c>
-      <c r="I6" t="str">
-        <v>Full Time</v>
-      </c>
-      <c r="J6" t="str">
-        <v>Onsite</v>
-      </c>
-      <c r="K6" t="str">
-        <v>https://southasiacareers.deloitte.com/job/Bengaluru-Technology-and-Transformation-EAD-AIML-Generative-AI-Analyst/46258444/</v>
+        <v>https://apply.workable.com/weekday-1/j/C7AA0742E4/</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:K6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:K2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>